<commit_message>
Zeitplan update + Vorwort verbesserung + Einleitung mit Leitfragen geschrieben
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TBZ\ABU\VA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E98EAD7-3BF1-4B07-BA5B-ED84C77FF084}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B9EDBF-E210-45A0-B344-893573D2DC4C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D613313E-A0B8-4535-9AFB-AF457A93B59D}"/>
+    <workbookView minimized="1" xWindow="2700" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{D613313E-A0B8-4535-9AFB-AF457A93B59D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Arbeitsschritte</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>2. Meilenstein 22.10.2019 (Alle Kapitel dokumentiert, Interview dokumentiert, fehlt nur noch die Abgabe der VA)</t>
+  </si>
+  <si>
+    <t>abgeschlossen</t>
   </si>
 </sst>
 </file>
@@ -294,23 +297,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,7 +635,7 @@
   <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,36 +649,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" s="5" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="11">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14"/>
+      <c r="F2" s="13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B3" s="6">
@@ -723,13 +728,13 @@
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
@@ -792,13 +797,13 @@
       <c r="F10" s="9"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="6">

</xml_diff>

<commit_message>
Einleitung angepasst, Vorwort rausgenommen, allgemeine korrekturen begonnen, Arbeitsprotokoll erneuert und Sitzungsprotokoll eingeführt
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TBZ\ABU\VA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mher.ASP\Documents\Schule\VA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6B8530-9456-42B1-8ED7-FB21BE39FE77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CE0AD3-3E4C-4702-8D58-91FF1FEC71CB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D613313E-A0B8-4535-9AFB-AF457A93B59D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D613313E-A0B8-4535-9AFB-AF457A93B59D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Arbeitsschritte</t>
   </si>
@@ -159,6 +157,9 @@
   </si>
   <si>
     <t>abgeschlossen, Interviewfragen konnten noch nicht bearbeitet werden, da ich die Antworten noch nicht erhalten habe.</t>
+  </si>
+  <si>
+    <t>abgeschlossen, Interviewantworten sind angekommen ich bin wieder in Zeitplanung.</t>
   </si>
 </sst>
 </file>
@@ -306,20 +307,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,20 +639,20 @@
   <dimension ref="B1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B6" sqref="B6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="44.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="1.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="4" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:6" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
@@ -668,7 +669,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B2" s="8">
         <v>1</v>
       </c>
@@ -681,11 +682,11 @@
       <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B3" s="5">
         <v>2</v>
       </c>
@@ -698,11 +699,11 @@
       <c r="E3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>3</v>
       </c>
@@ -715,11 +716,11 @@
       <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="5">
         <v>4</v>
       </c>
@@ -732,18 +733,20 @@
       <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="F5" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-    </row>
-    <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -756,9 +759,9 @@
       <c r="E7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -771,9 +774,9 @@
       <c r="E8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="F8" s="13"/>
+    </row>
+    <row r="9" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -786,9 +789,9 @@
       <c r="E9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F9" s="13"/>
+    </row>
+    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -801,18 +804,18 @@
       <c r="E10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>9</v>
       </c>
@@ -825,16 +828,16 @@
       <c r="E12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="F12" s="13"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>